<commit_message>
Updated the MiniGreenhouse with the trained LSTM model
</commit_message>
<xml_diff>
--- a/output/python-code-for-graphics/1-rewards-360steps/rewards_list_scheduled.xlsx
+++ b/output/python-code-for-graphics/1-rewards-360steps/rewards_list_scheduled.xlsx
@@ -5,17 +5,30 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frm19\OneDrive - Wageningen University &amp; Research\2. Thesis - Information Technology\3. Software Projects\mini-greenhouse-calibrator-model\output\scheduled-NN_GL_GRU_DRL_360steps_start15days_newModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frm19\OneDrive - Wageningen University &amp; Research\2. Thesis - Information Technology\3. Software Projects\mini-greenhouse-calibrator-model\output\python-code-for-graphics\1-rewards-360steps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D98B90-03F4-4126-AA92-7750B49AEDD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041046D2-FE33-401B-AE0A-FBB4910CDC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3350" yWindow="-14400" windowWidth="12800" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -391,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1445"/>
+  <dimension ref="A1:C1447"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A1420" workbookViewId="0">
+      <selection activeCell="B1446" sqref="B1446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16294,6 +16307,26 @@
         <v>9.0699190619747334</v>
       </c>
     </row>
+    <row r="1446" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B1446">
+        <f>AVERAGE(B2:B1445)</f>
+        <v>6.2811073836390131E-3</v>
+      </c>
+      <c r="C1446">
+        <f>AVERAGE(C2:C1445)</f>
+        <v>-5.9896571317258749</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B1447">
+        <f>STDEV(B2:B1445)</f>
+        <v>4.7167148310380616E-2</v>
+      </c>
+      <c r="C1447">
+        <f>STDEV(C2:C1445)</f>
+        <v>4.3740591250864922</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>